<commit_message>
f1 score + rearrange folders
</commit_message>
<xml_diff>
--- a/activity-protocol-CT.xlsx
+++ b/activity-protocol-CT.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Indy\Desktop\coding\Dementia_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/coding/Dementia_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CB9B6B-5993-429E-B1F7-B5064689A23C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A02A4C4-90B4-B742-9228-39AF75000AB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -283,7 +277,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,7 +320,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -604,22 +598,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G50" zoomScale="161" workbookViewId="0">
-      <selection activeCell="P83" sqref="P83"/>
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47:L85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -642,7 +636,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -656,7 +650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -670,7 +664,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -687,7 +681,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -701,12 +695,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -723,7 +717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -740,7 +734,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -757,7 +751,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -771,12 +765,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -790,7 +784,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -804,7 +798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -818,12 +812,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>13</v>
       </c>
@@ -840,7 +834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>14</v>
       </c>
@@ -857,7 +851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>15</v>
       </c>
@@ -874,7 +868,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>16</v>
       </c>
@@ -894,7 +888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17</v>
       </c>
@@ -914,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>18</v>
       </c>
@@ -934,7 +928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>19</v>
       </c>
@@ -951,7 +945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
@@ -968,7 +962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>21</v>
       </c>
@@ -982,7 +976,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>22</v>
       </c>
@@ -999,7 +993,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>23</v>
       </c>
@@ -1016,7 +1010,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>16</v>
       </c>
@@ -1033,7 +1027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>17</v>
       </c>
@@ -1050,7 +1044,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>18</v>
       </c>
@@ -1067,7 +1061,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>19</v>
       </c>
@@ -1084,7 +1078,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>20</v>
       </c>
@@ -1098,7 +1092,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1106,769 +1100,769 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="8:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <v>41.1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>65</v>
+      </c>
+      <c r="J47">
+        <f>H47/0.16</f>
+        <v>256.875</v>
+      </c>
+      <c r="K47">
+        <f>ROUND(J47,0)</f>
+        <v>257</v>
+      </c>
+      <c r="L47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <v>33.75</v>
+      </c>
+      <c r="I48" t="s">
+        <v>66</v>
+      </c>
+      <c r="J48">
+        <f t="shared" ref="J48:J85" si="0">H48/0.16</f>
+        <v>210.9375</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ref="K48:K85" si="1">ROUND(J48,0)</f>
+        <v>211</v>
+      </c>
+      <c r="L48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <v>34.14</v>
+      </c>
+      <c r="I49" t="s">
+        <v>65</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>213.375</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="1"/>
+        <v>213</v>
+      </c>
+      <c r="L49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <v>9.1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>67</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>56.875</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="L50" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <v>34.9</v>
+      </c>
+      <c r="I51" t="s">
+        <v>66</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>218.125</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="L51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>33.43</v>
+      </c>
+      <c r="I52" t="s">
+        <v>68</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="0"/>
+        <v>208.9375</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="1"/>
+        <v>209</v>
+      </c>
+      <c r="L52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>40.65</v>
+      </c>
+      <c r="I53" t="s">
+        <v>65</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="0"/>
+        <v>254.0625</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="1"/>
+        <v>254</v>
+      </c>
+      <c r="L53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="I54" t="s">
+        <v>68</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="0"/>
+        <v>212.62500000000003</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="1"/>
+        <v>213</v>
+      </c>
+      <c r="L54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <v>23.14</v>
+      </c>
+      <c r="I55" t="s">
+        <v>67</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="0"/>
+        <v>144.625</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>145</v>
+      </c>
+      <c r="L55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <v>32.520000000000003</v>
+      </c>
+      <c r="I56" t="s">
+        <v>65</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="0"/>
+        <v>203.25000000000003</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+      <c r="L56" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="I57" t="s">
+        <v>67</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="0"/>
+        <v>50.187499999999993</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="L57" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <v>30.66</v>
+      </c>
+      <c r="I58" t="s">
+        <v>69</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="0"/>
+        <v>191.625</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+      <c r="L58" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <v>46.66</v>
+      </c>
+      <c r="I59" t="s">
+        <v>70</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="0"/>
+        <v>291.625</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="1"/>
+        <v>292</v>
+      </c>
+      <c r="L59" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H60">
-        <v>41.1</v>
+        <v>36.15</v>
       </c>
       <c r="I60" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J60">
-        <f>H60/0.16</f>
-        <v>256.875</v>
+        <f t="shared" si="0"/>
+        <v>225.9375</v>
       </c>
       <c r="K60">
-        <f>ROUND(J60,0)</f>
-        <v>257</v>
+        <f t="shared" si="1"/>
+        <v>226</v>
       </c>
       <c r="L60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H61">
-        <v>33.75</v>
+        <v>47.68</v>
       </c>
       <c r="I61" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="J61">
-        <f t="shared" ref="J61:J98" si="0">H61/0.16</f>
-        <v>210.9375</v>
+        <f t="shared" si="0"/>
+        <v>298</v>
       </c>
       <c r="K61">
-        <f t="shared" ref="K61:K98" si="1">ROUND(J61,0)</f>
-        <v>211</v>
+        <f t="shared" si="1"/>
+        <v>298</v>
       </c>
       <c r="L61" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="8:12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H62">
-        <v>34.14</v>
+        <v>14.96</v>
       </c>
       <c r="I62" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J62">
         <f t="shared" si="0"/>
-        <v>213.375</v>
+        <v>93.5</v>
       </c>
       <c r="K62">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>94</v>
       </c>
       <c r="L62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="8:12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H63">
-        <v>9.1</v>
+        <v>15.98</v>
       </c>
       <c r="I63" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="J63">
         <f t="shared" si="0"/>
-        <v>56.875</v>
+        <v>99.875</v>
       </c>
       <c r="K63">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="L63" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="8:12">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H64">
-        <v>34.9</v>
+        <v>82.9</v>
       </c>
       <c r="I64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J64">
         <f t="shared" si="0"/>
-        <v>218.125</v>
+        <v>518.125</v>
       </c>
       <c r="K64">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>518</v>
       </c>
       <c r="L64" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="65" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H65">
-        <v>33.43</v>
+        <v>104.8</v>
       </c>
       <c r="I65" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="J65">
         <f t="shared" si="0"/>
-        <v>208.9375</v>
+        <v>655</v>
       </c>
       <c r="K65">
         <f t="shared" si="1"/>
-        <v>209</v>
+        <v>655</v>
       </c>
       <c r="L65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="8:12">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H66">
-        <v>40.65</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I66" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J66">
         <f t="shared" si="0"/>
-        <v>254.0625</v>
+        <v>233.12499999999997</v>
       </c>
       <c r="K66">
         <f t="shared" si="1"/>
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="L66" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H67">
-        <v>34.020000000000003</v>
+        <v>30.8</v>
       </c>
       <c r="I67" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="J67">
         <f t="shared" si="0"/>
-        <v>212.62500000000003</v>
+        <v>192.5</v>
       </c>
       <c r="K67">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="L67" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="68" spans="8:12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H68">
-        <v>23.14</v>
+        <v>58.3</v>
       </c>
       <c r="I68" t="s">
         <v>67</v>
       </c>
       <c r="J68">
         <f t="shared" si="0"/>
-        <v>144.625</v>
+        <v>364.375</v>
       </c>
       <c r="K68">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>364</v>
       </c>
       <c r="L68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="8:12">
+    <row r="69" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H69">
-        <v>32.520000000000003</v>
+        <v>43.16</v>
       </c>
       <c r="I69" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J69">
         <f t="shared" si="0"/>
-        <v>203.25000000000003</v>
+        <v>269.75</v>
       </c>
       <c r="K69">
         <f t="shared" si="1"/>
-        <v>203</v>
+        <v>270</v>
       </c>
       <c r="L69" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="8:12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H70">
-        <v>8.0299999999999994</v>
+        <v>40.31</v>
       </c>
       <c r="I70" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="J70">
         <f t="shared" si="0"/>
-        <v>50.187499999999993</v>
+        <v>251.9375</v>
       </c>
       <c r="K70">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>252</v>
       </c>
       <c r="L70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="8:12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H71">
-        <v>30.66</v>
+        <v>32.28</v>
       </c>
       <c r="I71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J71">
         <f t="shared" si="0"/>
-        <v>191.625</v>
+        <v>201.75</v>
       </c>
       <c r="K71">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="L71" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H72">
-        <v>46.66</v>
+        <v>12.5</v>
       </c>
       <c r="I72" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="J72">
         <f t="shared" si="0"/>
-        <v>291.625</v>
+        <v>78.125</v>
       </c>
       <c r="K72">
         <f t="shared" si="1"/>
-        <v>292</v>
+        <v>78</v>
       </c>
       <c r="L72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="8:12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H73">
-        <v>36.15</v>
+        <v>18.29</v>
       </c>
       <c r="I73" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="J73">
         <f t="shared" si="0"/>
-        <v>225.9375</v>
+        <v>114.31249999999999</v>
       </c>
       <c r="K73">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>114</v>
       </c>
       <c r="L73" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="74" spans="8:12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H74">
-        <v>47.68</v>
+        <v>20.13</v>
       </c>
       <c r="I74" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J74">
         <f t="shared" si="0"/>
-        <v>298</v>
+        <v>125.81249999999999</v>
       </c>
       <c r="K74">
         <f t="shared" si="1"/>
-        <v>298</v>
+        <v>126</v>
       </c>
       <c r="L74" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="75" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H75">
-        <v>14.96</v>
+        <v>24.58</v>
       </c>
       <c r="I75" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="J75">
         <f t="shared" si="0"/>
-        <v>93.5</v>
+        <v>153.625</v>
       </c>
       <c r="K75">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="L75" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="76" spans="8:12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="76" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H76">
-        <v>15.98</v>
+        <v>15.53</v>
       </c>
       <c r="I76" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="J76">
         <f t="shared" si="0"/>
-        <v>99.875</v>
+        <v>97.0625</v>
       </c>
       <c r="K76">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L76" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="8:12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H77">
-        <v>82.9</v>
+        <v>4.5</v>
       </c>
       <c r="I77" t="s">
         <v>67</v>
       </c>
       <c r="J77">
         <f t="shared" si="0"/>
-        <v>518.125</v>
+        <v>28.125</v>
       </c>
       <c r="K77">
         <f t="shared" si="1"/>
-        <v>518</v>
+        <v>28</v>
       </c>
       <c r="L77" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="8:12">
+    <row r="78" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H78">
-        <v>104.8</v>
+        <v>41.42</v>
       </c>
       <c r="I78" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J78">
         <f t="shared" si="0"/>
-        <v>655</v>
+        <v>258.875</v>
       </c>
       <c r="K78">
         <f t="shared" si="1"/>
-        <v>655</v>
+        <v>259</v>
       </c>
       <c r="L78" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H79">
-        <v>37.299999999999997</v>
+        <v>56.73</v>
       </c>
       <c r="I79" t="s">
         <v>67</v>
       </c>
       <c r="J79">
         <f t="shared" si="0"/>
-        <v>233.12499999999997</v>
+        <v>354.5625</v>
       </c>
       <c r="K79">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>355</v>
       </c>
       <c r="L79" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="8:12">
+    <row r="80" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H80">
-        <v>30.8</v>
+        <v>25.78</v>
       </c>
       <c r="I80" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="J80">
         <f t="shared" si="0"/>
-        <v>192.5</v>
+        <v>161.125</v>
       </c>
       <c r="K80">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="L80" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="8:12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H81">
-        <v>58.3</v>
+        <v>26.97</v>
       </c>
       <c r="I81" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J81">
         <f t="shared" si="0"/>
-        <v>364.375</v>
+        <v>168.5625</v>
       </c>
       <c r="K81">
         <f t="shared" si="1"/>
-        <v>364</v>
+        <v>169</v>
       </c>
       <c r="L81" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="8:12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H82">
-        <v>43.16</v>
+        <v>15.53</v>
       </c>
       <c r="I82" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J82">
         <f t="shared" si="0"/>
-        <v>269.75</v>
+        <v>97.0625</v>
       </c>
       <c r="K82">
         <f t="shared" si="1"/>
-        <v>270</v>
+        <v>97</v>
       </c>
       <c r="L82" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="8:12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="83" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H83">
-        <v>40.31</v>
+        <v>22.04</v>
       </c>
       <c r="I83" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J83">
         <f t="shared" si="0"/>
-        <v>251.9375</v>
+        <v>137.75</v>
       </c>
       <c r="K83">
         <f t="shared" si="1"/>
-        <v>252</v>
+        <v>138</v>
       </c>
       <c r="L83" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="84" spans="8:12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H84">
-        <v>32.28</v>
+        <v>21.75</v>
       </c>
       <c r="I84" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="J84">
         <f t="shared" si="0"/>
-        <v>201.75</v>
+        <v>135.9375</v>
       </c>
       <c r="K84">
         <f t="shared" si="1"/>
-        <v>202</v>
+        <v>136</v>
       </c>
       <c r="L84" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="85" spans="8:12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H85">
-        <v>12.5</v>
+        <v>3.25</v>
       </c>
       <c r="I85" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J85">
         <f t="shared" si="0"/>
-        <v>78.125</v>
+        <v>20.3125</v>
       </c>
       <c r="K85">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="L85" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="86" spans="8:12">
-      <c r="H86">
-        <v>18.29</v>
-      </c>
-      <c r="I86" t="s">
-        <v>77</v>
-      </c>
-      <c r="J86">
-        <f t="shared" si="0"/>
-        <v>114.31249999999999</v>
-      </c>
-      <c r="K86">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-      <c r="L86" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="87" spans="8:12">
-      <c r="H87">
-        <v>20.13</v>
-      </c>
-      <c r="I87" t="s">
-        <v>67</v>
-      </c>
-      <c r="J87">
-        <f t="shared" si="0"/>
-        <v>125.81249999999999</v>
-      </c>
-      <c r="K87">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-      <c r="L87" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="88" spans="8:12">
-      <c r="H88">
-        <v>24.58</v>
-      </c>
-      <c r="I88" t="s">
-        <v>78</v>
-      </c>
-      <c r="J88">
-        <f t="shared" si="0"/>
-        <v>153.625</v>
-      </c>
-      <c r="K88">
-        <f t="shared" si="1"/>
-        <v>154</v>
-      </c>
-      <c r="L88" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="89" spans="8:12">
-      <c r="H89">
-        <v>15.53</v>
-      </c>
-      <c r="I89" t="s">
-        <v>79</v>
-      </c>
-      <c r="J89">
-        <f t="shared" si="0"/>
-        <v>97.0625</v>
-      </c>
-      <c r="K89">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="L89" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="90" spans="8:12">
-      <c r="H90">
-        <v>4.5</v>
-      </c>
-      <c r="I90" t="s">
-        <v>67</v>
-      </c>
-      <c r="J90">
-        <f t="shared" si="0"/>
-        <v>28.125</v>
-      </c>
-      <c r="K90">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="L90" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="91" spans="8:12">
-      <c r="H91">
-        <v>41.42</v>
-      </c>
-      <c r="I91" t="s">
-        <v>67</v>
-      </c>
-      <c r="J91">
-        <f t="shared" si="0"/>
-        <v>258.875</v>
-      </c>
-      <c r="K91">
-        <f t="shared" si="1"/>
-        <v>259</v>
-      </c>
-      <c r="L91" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="8:12">
-      <c r="H92">
-        <v>56.73</v>
-      </c>
-      <c r="I92" t="s">
-        <v>67</v>
-      </c>
-      <c r="J92">
-        <f t="shared" si="0"/>
-        <v>354.5625</v>
-      </c>
-      <c r="K92">
-        <f t="shared" si="1"/>
-        <v>355</v>
-      </c>
-      <c r="L92" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="93" spans="8:12">
-      <c r="H93">
-        <v>25.78</v>
-      </c>
-      <c r="I93" t="s">
-        <v>80</v>
-      </c>
-      <c r="J93">
-        <f t="shared" si="0"/>
-        <v>161.125</v>
-      </c>
-      <c r="K93">
-        <f t="shared" si="1"/>
-        <v>161</v>
-      </c>
-      <c r="L93" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94" spans="8:12">
-      <c r="H94">
-        <v>26.97</v>
-      </c>
-      <c r="I94" t="s">
-        <v>81</v>
-      </c>
-      <c r="J94">
-        <f t="shared" si="0"/>
-        <v>168.5625</v>
-      </c>
-      <c r="K94">
-        <f t="shared" si="1"/>
-        <v>169</v>
-      </c>
-      <c r="L94" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="95" spans="8:12">
-      <c r="H95">
-        <v>15.53</v>
-      </c>
-      <c r="I95" t="s">
-        <v>67</v>
-      </c>
-      <c r="J95">
-        <f t="shared" si="0"/>
-        <v>97.0625</v>
-      </c>
-      <c r="K95">
-        <f t="shared" si="1"/>
-        <v>97</v>
-      </c>
-      <c r="L95" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="96" spans="8:12">
-      <c r="H96">
-        <v>22.04</v>
-      </c>
-      <c r="I96" t="s">
-        <v>80</v>
-      </c>
-      <c r="J96">
-        <f t="shared" si="0"/>
-        <v>137.75</v>
-      </c>
-      <c r="K96">
-        <f t="shared" si="1"/>
-        <v>138</v>
-      </c>
-      <c r="L96" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="97" spans="8:12">
-      <c r="H97">
-        <v>21.75</v>
-      </c>
-      <c r="I97" t="s">
-        <v>81</v>
-      </c>
-      <c r="J97">
-        <f t="shared" si="0"/>
-        <v>135.9375</v>
-      </c>
-      <c r="K97">
-        <f t="shared" si="1"/>
-        <v>136</v>
-      </c>
-      <c r="L97" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="98" spans="8:12">
-      <c r="H98">
-        <v>3.25</v>
-      </c>
-      <c r="I98" t="s">
-        <v>67</v>
-      </c>
-      <c r="J98">
-        <f t="shared" si="0"/>
-        <v>20.3125</v>
-      </c>
-      <c r="K98">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="L98" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>